<commit_message>
Added daily and weekly machine forecast hours to the spreadsheet  control in the Chart View tab.
Changed subject caption of tasks in Dept Schedule View.

Addresses Issue #162
</commit_message>
<xml_diff>
--- a/Toolroom Project Viewer/Resources/Forecasted_Hours.xlsx
+++ b/Toolroom Project Viewer/Resources/Forecasted_Hours.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smcltd-my.sharepoint.com/personal/joshua_meservey_smcltd_com/Documents/Visual Studio 2017/Projects/Toolroom Scheduler/Toolroom Project Viewer/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshua.meservey\OneDrive - SMC Ltd\Visual Studio 2017\Projects\Toolroom Scheduler\Toolroom Project Viewer\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_F68BC7C5D9093CA68ACFBA0609337A270BE173E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{125D945E-0397-4E9F-B675-2C2150DE59E4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE67460-51B8-4EE1-B570-06189EB73B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Weekly Hrs" sheetId="1" r:id="rId1"/>
-    <sheet name="Daily Hrs" sheetId="3" r:id="rId2"/>
+    <sheet name="Dept. Weekly Hrs" sheetId="1" r:id="rId1"/>
+    <sheet name="Dept. Daily Hrs" sheetId="3" r:id="rId2"/>
+    <sheet name="Mach. Weekly Hrs" sheetId="5" r:id="rId3"/>
+    <sheet name="Mach. Daily Hrs" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>Design</t>
   </si>
@@ -78,9 +80,6 @@
     <t>EDM Wire (In-House)</t>
   </si>
   <si>
-    <t>Forecasted Hours</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -88,6 +87,12 @@
   </si>
   <si>
     <t>Manual</t>
+  </si>
+  <si>
+    <t>Dept. Forecasted Hours</t>
+  </si>
+  <si>
+    <t>Mach. Forecasted Hours</t>
   </si>
 </sst>
 </file>
@@ -482,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +502,7 @@
     <row r="1" spans="1:22" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3"/>
       <c r="B1" s="9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -822,7 +827,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -918,7 +923,7 @@
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -942,7 +947,7 @@
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="6">
         <f>SUM(C4:C16)</f>
@@ -1036,7 +1041,7 @@
   <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1055,7 @@
     <row r="1" spans="1:22" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3"/>
       <c r="B1" s="9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1375,7 +1380,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1471,7 +1476,7 @@
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1495,7 +1500,7 @@
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="6">
         <f>SUM(C4:C16)</f>
@@ -1571,6 +1576,968 @@
       </c>
       <c r="U18" s="6">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:U1"/>
+    <mergeCell ref="B2:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D8B735-8D1B-4E81-88A3-513E3114602F}">
+  <dimension ref="A1:V16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="21" width="5.7109375" customWidth="1"/>
+    <col min="22" max="22" width="3.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3"/>
+      <c r="B1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="3"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2">
+        <v>9</v>
+      </c>
+      <c r="L2" s="2">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2">
+        <v>12</v>
+      </c>
+      <c r="O2" s="2">
+        <v>13</v>
+      </c>
+      <c r="P2" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>15</v>
+      </c>
+      <c r="R2" s="2">
+        <v>16</v>
+      </c>
+      <c r="S2" s="2">
+        <v>17</v>
+      </c>
+      <c r="T2" s="2">
+        <v>18</v>
+      </c>
+      <c r="U2" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="6">
+        <f>SUM(C4:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
+        <f>SUM(D4:D15)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="6">
+        <f>SUM(E4:E15)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <f>SUM(F4:F15)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <f>SUM(G4:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <f>SUM(H4:H15)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <f>SUM(I4:I15)</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <f>SUM(J4:J15)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <f>SUM(K4:K15)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <f>SUM(L4:L15)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="6">
+        <f>SUM(M4:M15)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="6">
+        <f>SUM(N4:N15)</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="6">
+        <f>SUM(O4:O15)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="6">
+        <f>SUM(P4:P15)</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6">
+        <f>SUM(Q4:Q15)</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="6">
+        <f>SUM(R4:R15)</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="6">
+        <f>SUM(S4:S15)</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="6">
+        <f>SUM(T4:T15)</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="6">
+        <f>SUM(U4:U15)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:U1"/>
+    <mergeCell ref="B2:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3C7D60-E8A8-4001-8EBB-5675982A6587}">
+  <dimension ref="A1:V16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="21" width="5.7109375" customWidth="1"/>
+    <col min="22" max="22" width="3.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3"/>
+      <c r="B1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="3"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2">
+        <v>9</v>
+      </c>
+      <c r="L2" s="2">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2">
+        <v>12</v>
+      </c>
+      <c r="O2" s="2">
+        <v>13</v>
+      </c>
+      <c r="P2" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>15</v>
+      </c>
+      <c r="R2" s="2">
+        <v>16</v>
+      </c>
+      <c r="S2" s="2">
+        <v>17</v>
+      </c>
+      <c r="T2" s="2">
+        <v>18</v>
+      </c>
+      <c r="U2" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="6">
+        <f>SUM(C4:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
+        <f>SUM(D4:D15)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="6">
+        <f>SUM(E4:E15)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <f>SUM(F4:F15)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <f>SUM(G4:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <f>SUM(H4:H15)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <f>SUM(I4:I15)</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <f>SUM(J4:J15)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <f>SUM(K4:K15)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <f>SUM(L4:L15)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="6">
+        <f>SUM(M4:M15)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="6">
+        <f>SUM(N4:N15)</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="6">
+        <f>SUM(O4:O15)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="6">
+        <f>SUM(P4:P15)</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="6">
+        <f>SUM(Q4:Q15)</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="6">
+        <f>SUM(R4:R15)</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="6">
+        <f>SUM(S4:S15)</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="6">
+        <f>SUM(T4:T15)</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="6">
+        <f>SUM(U4:U15)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>